<commit_message>
Update Chart of Accounts import/export functionality to correctly handle updates and ensure accurate data.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f5791d6d-82c7-4faa-bd4a-8030f920af85
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/80550fad-9a85-4035-aa54-a26530837091/3da0dcc3-fbc5-499d-85d8-1f2c0b0f1d8d.jpg
</commit_message>
<xml_diff>
--- a/test/data/coa-import/updated-tests/test-accounts-import-updated.xlsx
+++ b/test/data/coa-import/updated-tests/test-accounts-import-updated.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="CoA Import" sheetId="1" r:id="rId1"/>
+    <sheet name="Accounts" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,17 +397,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
         <v>AccountCode</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Name</v>
       </c>
       <c r="C1" t="str">
         <v>Type</v>
@@ -419,7 +419,7 @@
         <v>Description</v>
       </c>
       <c r="F1" t="str">
-        <v>ParentCode</v>
+        <v>Active</v>
       </c>
       <c r="G1" t="str">
         <v>IsSubledger</v>
@@ -427,13 +427,16 @@
       <c r="H1" t="str">
         <v>SubledgerType</v>
       </c>
+      <c r="I1" t="str">
+        <v>ParentId</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>10000</v>
+        <v>Cash and Cash Equivalents</v>
       </c>
       <c r="B2" t="str">
-        <v>ASSETS</v>
+        <v>10100</v>
       </c>
       <c r="C2" t="str">
         <v>ASSET</v>
@@ -442,24 +445,21 @@
         <v>Current</v>
       </c>
       <c r="E2" t="str">
-        <v>Assets Category</v>
-      </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="H2" t="str">
-        <v/>
+        <v>Cash and cash equivalent accounts</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>10100</v>
+        <v>Checking Account</v>
       </c>
       <c r="B3" t="str">
-        <v>Cash and Cash Equivalents</v>
+        <v>10101</v>
       </c>
       <c r="C3" t="str">
         <v>ASSET</v>
@@ -468,24 +468,24 @@
         <v>Current</v>
       </c>
       <c r="E3" t="str">
-        <v>Cash and equivalents</v>
-      </c>
-      <c r="F3" t="str">
-        <v>10000</v>
-      </c>
-      <c r="G3" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="H3" t="str">
-        <v/>
+        <v>Primary checking account</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>10100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>10101</v>
+        <v>Savings Account</v>
       </c>
       <c r="B4" t="str">
-        <v>Checking Account</v>
+        <v>10102</v>
       </c>
       <c r="C4" t="str">
         <v>ASSET</v>
@@ -494,24 +494,24 @@
         <v>Current</v>
       </c>
       <c r="E4" t="str">
-        <v>Main checking account</v>
-      </c>
-      <c r="F4" t="str">
+        <v>Business savings account</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>10100</v>
-      </c>
-      <c r="G4" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="H4" t="str">
-        <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>10102</v>
+        <v>Accounts Receivable</v>
       </c>
       <c r="B5" t="str">
-        <v>Savings Account</v>
+        <v>10200</v>
       </c>
       <c r="C5" t="str">
         <v>ASSET</v>
@@ -520,50 +520,47 @@
         <v>Current</v>
       </c>
       <c r="E5" t="str">
-        <v>Interest-bearing savings</v>
-      </c>
-      <c r="F5" t="str">
-        <v>10100</v>
-      </c>
-      <c r="G5" t="str">
-        <v>FALSE</v>
+        <v>Amounts owed by customers</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
       </c>
       <c r="H5" t="str">
-        <v/>
+        <v>Customer</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>10200</v>
+        <v>Long-term Investments</v>
       </c>
       <c r="B6" t="str">
-        <v>Accounts Receivable</v>
+        <v>10500</v>
       </c>
       <c r="C6" t="str">
         <v>ASSET</v>
       </c>
       <c r="D6" t="str">
-        <v>Current</v>
+        <v>NonCurrent</v>
       </c>
       <c r="E6" t="str">
-        <v>Money owed by customers</v>
-      </c>
-      <c r="F6" t="str">
-        <v>10000</v>
-      </c>
-      <c r="G6" t="str">
-        <v>TRUE</v>
-      </c>
-      <c r="H6" t="str">
-        <v>CUSTOMER</v>
+        <v>Investment accounts with terms &gt; 1 year</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>20000</v>
+        <v>Accounts Payable</v>
       </c>
       <c r="B7" t="str">
-        <v>LIABILITIES</v>
+        <v>20100</v>
       </c>
       <c r="C7" t="str">
         <v>LIABILITY</v>
@@ -572,229 +569,116 @@
         <v>Current</v>
       </c>
       <c r="E7" t="str">
-        <v>Liabilities Category</v>
-      </c>
-      <c r="F7" t="str">
-        <v/>
-      </c>
-      <c r="G7" t="str">
-        <v>FALSE</v>
+        <v>Amounts owed to vendors</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
       </c>
       <c r="H7" t="str">
-        <v/>
+        <v>Vendor</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>20100</v>
+        <v>Sales Revenue</v>
       </c>
       <c r="B8" t="str">
-        <v>Accounts Payable</v>
+        <v>40100</v>
       </c>
       <c r="C8" t="str">
-        <v>LIABILITY</v>
+        <v>REVENUE</v>
       </c>
       <c r="D8" t="str">
-        <v>Current</v>
+        <v>Operating</v>
       </c>
       <c r="E8" t="str">
-        <v>Money owed to suppliers</v>
-      </c>
-      <c r="F8" t="str">
-        <v>20000</v>
-      </c>
-      <c r="G8" t="str">
-        <v>TRUE</v>
-      </c>
-      <c r="H8" t="str">
-        <v>VENDOR</v>
+        <v>Income from primary business operations</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>30000</v>
+        <v>Direct Expenses</v>
       </c>
       <c r="B9" t="str">
-        <v>EQUITY</v>
+        <v>50100</v>
       </c>
       <c r="C9" t="str">
-        <v>EQUITY</v>
+        <v>EXPENSE</v>
       </c>
       <c r="D9" t="str">
-        <v>Retained Earnings</v>
+        <v>Operating</v>
       </c>
       <c r="E9" t="str">
-        <v>Equity Category</v>
-      </c>
-      <c r="F9" t="str">
-        <v/>
-      </c>
-      <c r="G9" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="H9" t="str">
-        <v/>
+        <v>Expenses directly tied to sales</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>40000</v>
+        <v>Indirect Expenses</v>
       </c>
       <c r="B10" t="str">
-        <v>REVENUE</v>
+        <v>50200</v>
       </c>
       <c r="C10" t="str">
-        <v>REVENUE</v>
+        <v>EXPENSE</v>
       </c>
       <c r="D10" t="str">
-        <v>Sales</v>
+        <v>Operating</v>
       </c>
       <c r="E10" t="str">
-        <v>Revenue Category</v>
-      </c>
-      <c r="F10" t="str">
-        <v/>
-      </c>
-      <c r="G10" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="H10" t="str">
-        <v/>
+        <v>Overhead expenses</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>40100</v>
+        <v>Utilities</v>
       </c>
       <c r="B11" t="str">
-        <v>Services Revenue</v>
+        <v>50300</v>
       </c>
       <c r="C11" t="str">
-        <v>REVENUE</v>
+        <v>EXPENSE</v>
       </c>
       <c r="D11" t="str">
-        <v>Sales</v>
+        <v>Operating</v>
       </c>
       <c r="E11" t="str">
-        <v>Services income</v>
-      </c>
-      <c r="F11" t="str">
-        <v>40000</v>
-      </c>
-      <c r="G11" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="H11" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>50000</v>
-      </c>
-      <c r="B12" t="str">
-        <v>EXPENSES</v>
-      </c>
-      <c r="C12" t="str">
-        <v>EXPENSE</v>
-      </c>
-      <c r="D12" t="str">
-        <v>Operating</v>
-      </c>
-      <c r="E12" t="str">
-        <v>Expenses Category</v>
-      </c>
-      <c r="F12" t="str">
-        <v/>
-      </c>
-      <c r="G12" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="H12" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>50100</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Rent Expense</v>
-      </c>
-      <c r="C13" t="str">
-        <v>EXPENSE</v>
-      </c>
-      <c r="D13" t="str">
-        <v>Operating</v>
-      </c>
-      <c r="E13" t="str">
-        <v>Office rent costs</v>
-      </c>
-      <c r="F13" t="str">
-        <v>50000</v>
-      </c>
-      <c r="G13" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="H13" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
+        <v>Updated utility expenses for facilities</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>50200</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Utilities Expense</v>
-      </c>
-      <c r="C14" t="str">
-        <v>EXPENSE</v>
-      </c>
-      <c r="D14" t="str">
-        <v>Operating</v>
-      </c>
-      <c r="E14" t="str">
-        <v>Utility costs</v>
-      </c>
-      <c r="F14" t="str">
-        <v>50000</v>
-      </c>
-      <c r="G14" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="H14" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>50300</v>
-      </c>
-      <c r="B15" t="str">
-        <v>Salaries Expense</v>
-      </c>
-      <c r="C15" t="str">
-        <v>EXPENSE</v>
-      </c>
-      <c r="D15" t="str">
-        <v>Operating</v>
-      </c>
-      <c r="E15" t="str">
-        <v>Employee salaries</v>
-      </c>
-      <c r="F15" t="str">
-        <v>50000</v>
-      </c>
-      <c r="G15" t="str">
-        <v>FALSE</v>
-      </c>
-      <c r="H15" t="str">
-        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>